<commit_message>
Add transactional prompt search and integrate Mode 3.1 into sample
Search 230K filtered WildChat prompts for Mode 3.1 (Transactional)
candidates using multi-pattern scoring heuristic. Results confirm
that real transactional prompts are extremely rare in WildChat:
- 100 candidates scored and reviewed → only 1 ACCEPT
- 99% rejected: most are utility (email drafting, 38%), advisory
  (product recommendations, 32%), or factual (technical, 20%)

The single ACCEPT ("reserve an additional family room for us")
replaces an overrepresented 1.3 prompt in high_gn block, bringing
Mode 3.1 count from 1 to 2. Pipeline regenerated successfully:
- Validation: passed (3.1 at 2, known WildChat gap)
- Baseline: 22 YES / 28 NO (sanity checks passed)
- Annotation spreadsheet: regenerated

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/output/annotation_spreadsheet.xlsx
+++ b/output/annotation_spreadsheet.xlsx
@@ -2165,10 +2165,7 @@
       </c>
       <c r="B36" s="16" t="inlineStr">
         <is>
-          <t>I am making a c++ sdl based game engine, currently doing the EventManager, I already make the classes and the event polling and notification using a pub/sub pattern. But in my first implementation I added a priority field to my base event, which I haven't even used yet, because I am unsure if this is really needed or not.
-In a typical game loop, you would process all events in the queue before updating the game state and rendering.
-If you process all events during each iteration, why would you need to prioritize some events?
-What do you think about this? I am wrong on this?</t>
+          <t>can you please reserve an additional family room for us. Please let me know the room rate as well. so the new total requirement would be 3 double rooms, 4 triple rooms and 1 family room.</t>
         </is>
       </c>
       <c r="C36" s="17" t="n"/>
@@ -2957,10 +2954,7 @@
       </c>
       <c r="B18" s="16" t="inlineStr">
         <is>
-          <t>I am making a c++ sdl based game engine, currently doing the EventManager, I already make the classes and the event polling and notification using a pub/sub pattern. But in my first implementation I added a priority field to my base event, which I haven't even used yet, because I am unsure if this is really needed or not.
-In a typical game loop, you would process all events in the queue before updating the game state and rendering.
-If you process all events during each iteration, why would you need to prioritize some events?
-What do you think about this? I am wrong on this?</t>
+          <t>can you please reserve an additional family room for us. Please let me know the room rate as well. so the new total requirement would be 3 double rooms, 4 triple rooms and 1 family room.</t>
         </is>
       </c>
       <c r="C18" s="17" t="n"/>
@@ -3844,7 +3838,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>unknown_entity:jordan,north carolina</t>
+          <t>unknown_entity:north carolina,jordan</t>
         </is>
       </c>
     </row>
@@ -3882,7 +3876,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>unknown_entity:TTS,Mimi,Phrase</t>
+          <t>unknown_entity:Mimi,Phrase,TTS</t>
         </is>
       </c>
     </row>
@@ -4050,7 +4044,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>temporal:2024; unknown_entity:Analog,Channel 4</t>
+          <t>temporal:2024; unknown_entity:Channel 4,Analog</t>
         </is>
       </c>
     </row>
@@ -4109,7 +4103,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>temporal:2024; unknown_entity:Laak,ana smith,Belisario Village</t>
+          <t>temporal:2024; unknown_entity:Avancena St.,ana smith,Davao City</t>
         </is>
       </c>
     </row>
@@ -4129,7 +4123,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>temporal:today; volatility:weather; unknown_entity:Keolis MHI,the British Market Briefing,Wallace Weatherill</t>
+          <t>temporal:today; volatility:weather; unknown_entity:the British Market Briefing,Wallace Weatherill,Keolis MHI</t>
         </is>
       </c>
     </row>
@@ -4225,7 +4219,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>temporal:current; unknown_entity:Building &amp; Real Estates,Assess</t>
+          <t>temporal:current; unknown_entity:Assess,Building &amp; Real Estates</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4295,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>unknown_entity:PHD,US,Biostatistics or Statistics</t>
+          <t>unknown_entity:US,Biostatistics or Statistics,PHD</t>
         </is>
       </c>
     </row>
@@ -4369,19 +4363,14 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>I am making a c++ sdl based game engine, currently doing the EventManager, I already make the classes and the event polling and notification using a pub/sub pattern. But in my first implementation I added a priority field to my base event, which I haven't even used yet, because I am unsure if this is really needed or not.
-In a typical game loop, you would process all events in the queue before updating the game state and rendering.
-If you process all events during each iteration, why would you need to prioritize some events?
-What do you think about this? I am wrong on this?</t>
+          <t>can you please reserve an additional family room for us. Please let me know the room rate as well. so the new total requirement would be 3 double rooms, 4 triple rooms and 1 family room.</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>temporal:current,currently; volatility:poll; unknown_entity:EventManager</t>
-        </is>
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v/>
       </c>
     </row>
     <row r="36">
@@ -4427,7 +4416,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>temporal:current; unknown_entity:B11,B10,BKK20230060010</t>
+          <t>temporal:current; unknown_entity:BKK20230060010,B11,B10</t>
         </is>
       </c>
     </row>
@@ -4651,7 +4640,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>unknown_entity:Albania,the United States,West Germany</t>
+          <t>unknown_entity:US,USSR,Yugoslavia</t>
         </is>
       </c>
     </row>
@@ -4671,7 +4660,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>unknown_entity:Wellington,YouTube,Auckland (The Rock</t>
+          <t>unknown_entity:Waikato (Coast,Magic,Hamilton</t>
         </is>
       </c>
     </row>
@@ -5711,11 +5700,11 @@
         <v/>
       </c>
       <c r="E38" t="n">
-        <v>1.3</v>
+        <v>3.1</v>
       </c>
       <c r="F38" s="21" t="inlineStr">
         <is>
-          <t>Review-accepted (1.3) from candidate_high_gn.csv.</t>
+          <t>Transactional (3.1) from dedicated WildChat search. Replaces overrepresented 1.3 in high_gn.</t>
         </is>
       </c>
     </row>

</xml_diff>